<commit_message>
Update Mobilitiy KPIs data
</commit_message>
<xml_diff>
--- a/public/files/MOV_SOC_REGIONAL.xlsx
+++ b/public/files/MOV_SOC_REGIONAL.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriela/Documents/2019/2019CADSALUD/CEEY/ATLAS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriela/Documents/2019/2019CADSALUD/CEEY/ATLAS/JULIO/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
     <sheet name="Diccionario" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
   <si>
     <t>sexo</t>
   </si>
@@ -118,42 +118,8 @@
     <t>Categórico</t>
   </si>
   <si>
-    <t xml:space="preserve">Movilidad intergeneracional en salud - Persistencia quintil I - Porcentaje de personas que al igual que sus padres permanecen al quintil más bajo de salud </t>
-  </si>
-  <si>
-    <t>Movilidad intergeneracional en salud - Persistencia quintil V- Porcentaje de personas que al igual que sus padres permanecen al quintil más alto de salud</t>
-  </si>
-  <si>
     <t>Movilidad intergeneracional en salud - Movilidad del quintil I a quintil V
 - Porcentaje de personas que nacieron en hogares del quintil I de salud y alcanzaron el quintil V.</t>
-  </si>
-  <si>
-    <t>Movilidad intergeneracional en educación - Persistencia nivel educativo sin estudios - Porcentaje de personas que al igual que su padre continúa sin estudios</t>
-  </si>
-  <si>
-    <t>Movilidad intergeneracional en educación - Persistencia nivel educativo carrera profesional - Porcentaje de personas que al igual que su padre cuentan con carrera profesional</t>
-  </si>
-  <si>
-    <t>Movilidad intergeneracional en educación - Movilidad del nivel educativo más bajo al más alto - Porcentaje de personas que cuentan con carrera profesional y que su padre no cuenta con estudios</t>
-  </si>
-  <si>
-    <t>Movilidad intergeneracional ocupacional - Persistencia trabajo agrícola - Porcentaje de personas que al igual que su padre tiene un trabajo agrícola</t>
-  </si>
-  <si>
-    <t>Movilidad intergeneracional ocupacional - Persistencia trabajo no manual de alta calificación - Porcentaje de personas que al igual que su padre cuentan con trabajo no manual de alta calificación.</t>
-  </si>
-  <si>
-    <t>Movilidad intergeneracional ocupacional - Movilidad de la ocupación menos calificada a la más calificada - Porcentaje de personas que cuentan con trabajo no manual de alta calificación y que su padre contaba con trabajo agrícola</t>
-  </si>
-  <si>
-    <t>Movilidad intergeneracional socioeconómica - Persistencia quintil I - Porcentaje de personas que al igual que sus padres permanecen al quintil más bajo del índice de riqueza</t>
-  </si>
-  <si>
-    <t>Movilidad intergeneracional socioeconómica - Persistencia quintil V - Porcentaje de personas que al igual que sus padres permanecen al quintil más alto del índice de riqueza</t>
-  </si>
-  <si>
-    <t>Movilidad intergeneracional socioeconómica - Movilidad del quintil I a quintil V
-Porcentaje de personas que nacieron en hogares del quintil I del índice de riqueza y alcanzaron el quintil V</t>
   </si>
   <si>
     <t>Nacional 
@@ -167,7 +133,38 @@
     <t>Cuantitativa-Porcentaje</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>Movilidad intergeneracional en educación - Movilidad del nivel educativo más bajo al más alto - Porcentaje de personas que cuentan con carrera profesional y cuyos padres tienen primaria o menos.</t>
+  </si>
+  <si>
+    <t>Movilidad intergeneracional socioeconómica - Persistencia quintil I - ”: Porcentaje de personas que al igual que sus padres permanecieron en el quintil más bajo del índice socioeconómico.</t>
+  </si>
+  <si>
+    <t>Movilidad intergeneracional socioeconómica - Persistencia quintil V - Porcentaje de personas que al igual que sus padres permanecieron en el quintil más alto del índice de socioeconómico.</t>
+  </si>
+  <si>
+    <t>Movilidad intergeneracional socioeconómica - Movilidad del quintil I a quintil V
+Porcentaje de personas que nacieron en hogares del quintil I del índice socioeconómico y alcanzaron el quintil V.</t>
+  </si>
+  <si>
+    <t>Movilidad intergeneracional en salud - Persistencia quintil I - Porcentaje de personas que al igual que sus padres permanecieron en el quintil más bajo del índice de salud.</t>
+  </si>
+  <si>
+    <t>Movilidad intergeneracional en educación - Persistencia nivel educativo carrera profesional - Porcentaje de personas que al igual que su padre cuentan con carrera profesional.</t>
+  </si>
+  <si>
+    <t>Movilidad intergeneracional en salud - Persistencia quintil V- Porcentaje de personas que al igual que sus padres permanecieron en el quintil más alto del índice de salud.</t>
+  </si>
+  <si>
+    <t>Movilidad intergeneracional en educación - Persistencia nivel educativo primaria - Porcentaje de personas que nacieron en hogares del quintil I del índice de salud y alcanzaron el quintil V.</t>
+  </si>
+  <si>
+    <t>Movilidad intergeneracional ocupacional - Persistencia trabajo agrícola - Porcentaje de personas que al igual que sus padres tienen un trabajo agrícola.</t>
+  </si>
+  <si>
+    <t>Movilidad intergeneracional ocupacional - Persistencia trabajo no manual de alta calificación - Porcentaje de personas que al igual que sus padres tienen un trabajo no manual de alta calificación.</t>
+  </si>
+  <si>
+    <t>Movilidad intergeneracional ocupacional - Movilidad de la ocupación menos calificada a la más calificada - Porcentaje de personas que tienen un trabajo no manual de alta calificación y cuyos padres tenían un trabajo agrícola.</t>
   </si>
 </sst>
 </file>
@@ -211,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -221,6 +218,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,11 +497,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -560,41 +557,41 @@
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C2">
-        <v>55</v>
-      </c>
-      <c r="D2">
-        <v>48</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>64</v>
-      </c>
-      <c r="H2">
-        <v>9</v>
-      </c>
-      <c r="I2">
-        <v>22</v>
-      </c>
-      <c r="J2">
-        <v>34</v>
-      </c>
-      <c r="K2">
-        <v>3</v>
-      </c>
-      <c r="L2">
-        <v>47</v>
-      </c>
-      <c r="M2">
-        <v>54</v>
-      </c>
-      <c r="N2">
-        <v>3</v>
+      <c r="C2" s="5">
+        <v>55.45</v>
+      </c>
+      <c r="D2" s="5">
+        <v>48.38</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1.84</v>
+      </c>
+      <c r="F2" s="5">
+        <v>36.78</v>
+      </c>
+      <c r="G2" s="5">
+        <v>63.51</v>
+      </c>
+      <c r="H2" s="5">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="I2" s="5">
+        <v>22.16</v>
+      </c>
+      <c r="J2" s="5">
+        <v>34.090000000000003</v>
+      </c>
+      <c r="K2" s="5">
+        <v>3.25</v>
+      </c>
+      <c r="L2" s="5">
+        <v>49.04</v>
+      </c>
+      <c r="M2" s="5">
+        <v>56.87</v>
+      </c>
+      <c r="N2" s="5">
+        <v>3.42</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -604,41 +601,41 @@
       <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="C3">
-        <v>58</v>
-      </c>
-      <c r="D3">
-        <v>43</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>53</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="I3">
-        <v>18</v>
-      </c>
-      <c r="J3">
-        <v>26</v>
-      </c>
-      <c r="K3">
-        <v>6</v>
-      </c>
-      <c r="L3">
-        <v>25</v>
-      </c>
-      <c r="M3">
-        <v>50</v>
-      </c>
-      <c r="N3">
-        <v>6</v>
+      <c r="C3" s="5">
+        <v>57.65</v>
+      </c>
+      <c r="D3" s="5">
+        <v>43.21</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2.75</v>
+      </c>
+      <c r="F3" s="5">
+        <v>28.77</v>
+      </c>
+      <c r="G3" s="5">
+        <v>52.55</v>
+      </c>
+      <c r="H3" s="5">
+        <v>10.45</v>
+      </c>
+      <c r="I3" s="5">
+        <v>17.7</v>
+      </c>
+      <c r="J3" s="5">
+        <v>25.59</v>
+      </c>
+      <c r="K3" s="5">
+        <v>5.75</v>
+      </c>
+      <c r="L3" s="5">
+        <v>23.35</v>
+      </c>
+      <c r="M3" s="5">
+        <v>49.1</v>
+      </c>
+      <c r="N3" s="5">
+        <v>7.83</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -648,41 +645,41 @@
       <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4">
-        <v>45</v>
-      </c>
-      <c r="D4">
-        <v>53</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>65</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4">
-        <v>25</v>
-      </c>
-      <c r="J4">
-        <v>24</v>
-      </c>
-      <c r="K4">
-        <v>4</v>
-      </c>
-      <c r="L4">
-        <v>25</v>
-      </c>
-      <c r="M4">
-        <v>43</v>
-      </c>
-      <c r="N4">
-        <v>6</v>
+      <c r="C4" s="5">
+        <v>45.42</v>
+      </c>
+      <c r="D4" s="5">
+        <v>53.48</v>
+      </c>
+      <c r="E4" s="5">
+        <v>3.14</v>
+      </c>
+      <c r="F4" s="5">
+        <v>35.93</v>
+      </c>
+      <c r="G4" s="5">
+        <v>65.069999999999993</v>
+      </c>
+      <c r="H4" s="5">
+        <v>10.36</v>
+      </c>
+      <c r="I4" s="5">
+        <v>25.36</v>
+      </c>
+      <c r="J4" s="5">
+        <v>23.89</v>
+      </c>
+      <c r="K4" s="5">
+        <v>4.16</v>
+      </c>
+      <c r="L4" s="5">
+        <v>26.47</v>
+      </c>
+      <c r="M4" s="5">
+        <v>45.51</v>
+      </c>
+      <c r="N4" s="5">
+        <v>5.18</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -692,41 +689,41 @@
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5">
-        <v>55</v>
-      </c>
-      <c r="D5">
-        <v>50</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>63</v>
-      </c>
-      <c r="H5">
-        <v>8</v>
-      </c>
-      <c r="I5">
-        <v>21</v>
-      </c>
-      <c r="J5">
-        <v>29</v>
-      </c>
-      <c r="K5">
-        <v>3</v>
-      </c>
-      <c r="L5">
-        <v>31</v>
-      </c>
-      <c r="M5">
-        <v>47</v>
-      </c>
-      <c r="N5">
-        <v>3</v>
+      <c r="C5" s="5">
+        <v>54.96</v>
+      </c>
+      <c r="D5" s="5">
+        <v>49.68</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1.63</v>
+      </c>
+      <c r="F5" s="5">
+        <v>43.83</v>
+      </c>
+      <c r="G5" s="5">
+        <v>62.59</v>
+      </c>
+      <c r="H5" s="5">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I5" s="5">
+        <v>21.4</v>
+      </c>
+      <c r="J5" s="5">
+        <v>28.85</v>
+      </c>
+      <c r="K5" s="5">
+        <v>3.15</v>
+      </c>
+      <c r="L5" s="5">
+        <v>29.35</v>
+      </c>
+      <c r="M5" s="5">
+        <v>49.45</v>
+      </c>
+      <c r="N5" s="5">
+        <v>3.2</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -736,41 +733,41 @@
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6">
-        <v>51</v>
-      </c>
-      <c r="D6">
-        <v>54</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>68</v>
-      </c>
-      <c r="H6">
-        <v>9</v>
-      </c>
-      <c r="I6">
-        <v>20</v>
-      </c>
-      <c r="J6">
-        <v>39</v>
-      </c>
-      <c r="K6">
-        <v>5</v>
-      </c>
-      <c r="L6">
-        <v>40</v>
-      </c>
-      <c r="M6">
-        <v>62</v>
-      </c>
-      <c r="N6">
-        <v>5</v>
+      <c r="C6" s="5">
+        <v>51.48</v>
+      </c>
+      <c r="D6" s="5">
+        <v>53.58</v>
+      </c>
+      <c r="E6" s="5">
+        <v>1.26</v>
+      </c>
+      <c r="F6" s="5">
+        <v>30.07</v>
+      </c>
+      <c r="G6" s="5">
+        <v>67.819999999999993</v>
+      </c>
+      <c r="H6" s="5">
+        <v>9.31</v>
+      </c>
+      <c r="I6" s="5">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="J6" s="5">
+        <v>38.57</v>
+      </c>
+      <c r="K6" s="5">
+        <v>4.7</v>
+      </c>
+      <c r="L6" s="5">
+        <v>37.58</v>
+      </c>
+      <c r="M6" s="5">
+        <v>65.25</v>
+      </c>
+      <c r="N6" s="5">
+        <v>3.98</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -780,41 +777,41 @@
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7">
-        <v>64</v>
-      </c>
-      <c r="D7">
-        <v>35</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>8</v>
-      </c>
-      <c r="G7">
-        <v>62</v>
-      </c>
-      <c r="H7">
-        <v>8</v>
-      </c>
-      <c r="I7">
-        <v>24</v>
-      </c>
-      <c r="J7">
-        <v>30</v>
-      </c>
-      <c r="K7">
-        <v>2</v>
-      </c>
-      <c r="L7">
-        <v>62</v>
-      </c>
-      <c r="M7">
-        <v>41</v>
-      </c>
-      <c r="N7">
-        <v>2</v>
+      <c r="C7" s="5">
+        <v>63.62</v>
+      </c>
+      <c r="D7" s="5">
+        <v>35.090000000000003</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1.91</v>
+      </c>
+      <c r="F7" s="5">
+        <v>44.97</v>
+      </c>
+      <c r="G7" s="5">
+        <v>61.63</v>
+      </c>
+      <c r="H7" s="5">
+        <v>7.87</v>
+      </c>
+      <c r="I7" s="5">
+        <v>24.38</v>
+      </c>
+      <c r="J7" s="5">
+        <v>29.91</v>
+      </c>
+      <c r="K7" s="5">
+        <v>1.65</v>
+      </c>
+      <c r="L7" s="5">
+        <v>66.72</v>
+      </c>
+      <c r="M7" s="5">
+        <v>58.24</v>
+      </c>
+      <c r="N7" s="5">
+        <v>2.29</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -824,41 +821,41 @@
       <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C8">
-        <v>42</v>
-      </c>
-      <c r="D8">
-        <v>83</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8">
-        <v>8</v>
-      </c>
-      <c r="J8">
-        <v>33</v>
-      </c>
-      <c r="K8">
-        <v>2</v>
-      </c>
-      <c r="L8">
-        <v>47</v>
-      </c>
-      <c r="M8">
-        <v>50</v>
-      </c>
-      <c r="N8">
-        <v>2</v>
+      <c r="C8" s="5">
+        <v>42.39</v>
+      </c>
+      <c r="D8" s="5">
+        <v>83.28</v>
+      </c>
+      <c r="E8" s="5">
+        <v>3.38</v>
+      </c>
+      <c r="F8" s="5">
+        <v>38.68</v>
+      </c>
+      <c r="G8" s="5">
+        <v>60.63</v>
+      </c>
+      <c r="H8" s="5">
+        <v>7.25</v>
+      </c>
+      <c r="I8" s="5">
+        <v>8.41</v>
+      </c>
+      <c r="J8" s="5">
+        <v>32.76</v>
+      </c>
+      <c r="K8" s="5">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="L8" s="5">
+        <v>48.98</v>
+      </c>
+      <c r="M8" s="5">
+        <v>55.77</v>
+      </c>
+      <c r="N8" s="5">
+        <v>2.58</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -868,42 +865,84 @@
       <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="C9">
-        <v>71</v>
-      </c>
-      <c r="D9">
-        <v>16</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9">
-        <v>30</v>
-      </c>
-      <c r="J9">
-        <v>35</v>
-      </c>
-      <c r="K9">
-        <v>4</v>
-      </c>
-      <c r="L9">
-        <v>46</v>
-      </c>
-      <c r="M9">
-        <v>57</v>
-      </c>
-      <c r="N9">
-        <v>5</v>
-      </c>
+      <c r="C9" s="5">
+        <v>70.86</v>
+      </c>
+      <c r="D9" s="5">
+        <v>16.170000000000002</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="F9" s="5">
+        <v>34.6</v>
+      </c>
+      <c r="G9" s="5">
+        <v>66.06</v>
+      </c>
+      <c r="H9" s="5">
+        <v>10.9</v>
+      </c>
+      <c r="I9" s="5">
+        <v>29.61</v>
+      </c>
+      <c r="J9" s="5">
+        <v>34.97</v>
+      </c>
+      <c r="K9" s="5">
+        <v>3.91</v>
+      </c>
+      <c r="L9" s="5">
+        <v>49.12</v>
+      </c>
+      <c r="M9" s="5">
+        <v>57.81</v>
+      </c>
+      <c r="N9" s="5">
+        <v>4.47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -949,7 +988,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>28</v>
@@ -960,10 +999,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -971,10 +1010,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -982,21 +1021,21 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -1004,10 +1043,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -1015,10 +1054,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -1026,10 +1065,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -1037,10 +1076,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -1048,10 +1087,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -1059,10 +1098,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -1070,10 +1109,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -1081,10 +1120,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>